<commit_message>
Release blancoRestGeneratorTs 0.1.0 !
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiSample.xlsx
+++ b/meta/api/BlancoApiSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E9577A-CA4E-5C42-8114-5775D44F2284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED93A97-0D1E-BE42-88DD-1D2E791E8376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="460" windowWidth="21420" windowHeight="17820" tabRatio="860" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="220">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -3135,7 +3135,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3549,6 +3549,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -4096,8 +4105,8 @@
   </sheetPr>
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4152,11 +4161,11 @@
       <c r="H5" s="96"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="136" t="s">
+      <c r="A6" s="190" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
+      <c r="B6" s="191"/>
+      <c r="C6" s="192"/>
       <c r="D6" s="134" t="s">
         <v>166</v>
       </c>
@@ -5422,8 +5431,8 @@
   </sheetPr>
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD23"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -6069,7 +6078,9 @@
         <v>141</v>
       </c>
       <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
+      <c r="I41" s="24" t="s">
+        <v>141</v>
+      </c>
       <c r="J41" s="24">
         <v>0</v>
       </c>
@@ -6099,7 +6110,9 @@
       <c r="F42" s="25"/>
       <c r="G42" s="86"/>
       <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
+      <c r="I42" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J42" s="21"/>
       <c r="K42" s="31"/>
       <c r="L42" s="21">
@@ -6129,7 +6142,9 @@
       <c r="H43" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I43" s="25"/>
+      <c r="I43" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J43" s="21"/>
       <c r="K43" s="31"/>
       <c r="L43" s="21"/>
@@ -6153,7 +6168,9 @@
       <c r="F44" s="82"/>
       <c r="G44" s="88"/>
       <c r="H44" s="82"/>
-      <c r="I44" s="25"/>
+      <c r="I44" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J44" s="21"/>
       <c r="K44" s="31"/>
       <c r="L44" s="21"/>
@@ -6179,7 +6196,9 @@
       <c r="F45" s="26"/>
       <c r="G45" s="87"/>
       <c r="H45" s="26"/>
-      <c r="I45" s="25"/>
+      <c r="I45" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J45" s="25"/>
       <c r="K45" s="32"/>
       <c r="L45" s="25"/>
@@ -6205,7 +6224,9 @@
       <c r="F46" s="26"/>
       <c r="G46" s="87"/>
       <c r="H46" s="26"/>
-      <c r="I46" s="25"/>
+      <c r="I46" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J46" s="21"/>
       <c r="K46" s="31"/>
       <c r="L46" s="21"/>
@@ -6229,7 +6250,9 @@
       <c r="F47" s="26"/>
       <c r="G47" s="87"/>
       <c r="H47" s="26"/>
-      <c r="I47" s="25"/>
+      <c r="I47" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J47" s="21"/>
       <c r="K47" s="31"/>
       <c r="L47" s="21"/>
@@ -6610,8 +6633,8 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="S42" sqref="G42:S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -7214,7 +7237,9 @@
         <v>141</v>
       </c>
       <c r="H38" s="67"/>
-      <c r="I38" s="24"/>
+      <c r="I38" s="24" t="s">
+        <v>141</v>
+      </c>
       <c r="J38" s="67"/>
       <c r="K38" s="67"/>
       <c r="L38" s="67"/>
@@ -7239,7 +7264,9 @@
       <c r="F39" s="67"/>
       <c r="G39" s="90"/>
       <c r="H39" s="67"/>
-      <c r="I39" s="25"/>
+      <c r="I39" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J39" s="65"/>
       <c r="K39" s="65"/>
       <c r="L39" s="65"/>
@@ -7262,7 +7289,9 @@
       <c r="F40" s="70"/>
       <c r="G40" s="91"/>
       <c r="H40" s="70"/>
-      <c r="I40" s="25"/>
+      <c r="I40" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J40" s="65"/>
       <c r="K40" s="65"/>
       <c r="L40" s="65"/>
@@ -7285,7 +7314,9 @@
       <c r="F41" s="74"/>
       <c r="G41" s="94"/>
       <c r="H41" s="74"/>
-      <c r="I41" s="25"/>
+      <c r="I41" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J41" s="65"/>
       <c r="K41" s="65"/>
       <c r="L41" s="65"/>
@@ -7310,7 +7341,9 @@
       <c r="F42" s="74"/>
       <c r="G42" s="92"/>
       <c r="H42" s="74"/>
-      <c r="I42" s="25"/>
+      <c r="I42" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J42" s="67"/>
       <c r="K42" s="67"/>
       <c r="L42" s="67"/>
@@ -7333,7 +7366,9 @@
       <c r="F43" s="74"/>
       <c r="G43" s="92"/>
       <c r="H43" s="74"/>
-      <c r="I43" s="25"/>
+      <c r="I43" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J43" s="65"/>
       <c r="K43" s="65"/>
       <c r="L43" s="65"/>
@@ -7356,7 +7391,9 @@
       <c r="F44" s="74"/>
       <c r="G44" s="92"/>
       <c r="H44" s="74"/>
-      <c r="I44" s="25"/>
+      <c r="I44" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J44" s="65"/>
       <c r="K44" s="65"/>
       <c r="L44" s="65"/>
@@ -7730,8 +7767,8 @@
   </sheetPr>
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD23"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -8377,7 +8414,9 @@
         <v>141</v>
       </c>
       <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
+      <c r="I41" s="24" t="s">
+        <v>141</v>
+      </c>
       <c r="J41" s="24">
         <v>0</v>
       </c>
@@ -8407,7 +8446,9 @@
       <c r="F42" s="25"/>
       <c r="G42" s="86"/>
       <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
+      <c r="I42" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J42" s="21"/>
       <c r="K42" s="31"/>
       <c r="L42" s="21">
@@ -8437,7 +8478,9 @@
       <c r="H43" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I43" s="25"/>
+      <c r="I43" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J43" s="21"/>
       <c r="K43" s="31"/>
       <c r="L43" s="21"/>
@@ -8461,7 +8504,9 @@
       <c r="F44" s="82"/>
       <c r="G44" s="88"/>
       <c r="H44" s="82"/>
-      <c r="I44" s="25"/>
+      <c r="I44" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J44" s="21"/>
       <c r="K44" s="31"/>
       <c r="L44" s="21"/>
@@ -8487,7 +8532,9 @@
       <c r="F45" s="26"/>
       <c r="G45" s="87"/>
       <c r="H45" s="26"/>
-      <c r="I45" s="25"/>
+      <c r="I45" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J45" s="25"/>
       <c r="K45" s="32"/>
       <c r="L45" s="25"/>
@@ -8513,7 +8560,9 @@
       <c r="F46" s="26"/>
       <c r="G46" s="87"/>
       <c r="H46" s="26"/>
-      <c r="I46" s="25"/>
+      <c r="I46" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J46" s="21"/>
       <c r="K46" s="31"/>
       <c r="L46" s="21"/>
@@ -8537,7 +8586,9 @@
       <c r="F47" s="26"/>
       <c r="G47" s="87"/>
       <c r="H47" s="26"/>
-      <c r="I47" s="25"/>
+      <c r="I47" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J47" s="21"/>
       <c r="K47" s="31"/>
       <c r="L47" s="21"/>
@@ -8922,7 +8973,7 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD20"/>
+      <selection activeCell="I38" sqref="I38:I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9525,7 +9576,9 @@
         <v>141</v>
       </c>
       <c r="H38" s="67"/>
-      <c r="I38" s="24"/>
+      <c r="I38" s="24" t="s">
+        <v>141</v>
+      </c>
       <c r="J38" s="67"/>
       <c r="K38" s="67"/>
       <c r="L38" s="67"/>
@@ -9550,7 +9603,9 @@
       <c r="F39" s="67"/>
       <c r="G39" s="90"/>
       <c r="H39" s="67"/>
-      <c r="I39" s="25"/>
+      <c r="I39" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J39" s="65"/>
       <c r="K39" s="65"/>
       <c r="L39" s="65"/>
@@ -9573,7 +9628,9 @@
       <c r="F40" s="70"/>
       <c r="G40" s="91"/>
       <c r="H40" s="70"/>
-      <c r="I40" s="25"/>
+      <c r="I40" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J40" s="65"/>
       <c r="K40" s="65"/>
       <c r="L40" s="65"/>
@@ -9596,7 +9653,9 @@
       <c r="F41" s="74"/>
       <c r="G41" s="94"/>
       <c r="H41" s="74"/>
-      <c r="I41" s="25"/>
+      <c r="I41" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J41" s="65"/>
       <c r="K41" s="65"/>
       <c r="L41" s="65"/>
@@ -9621,7 +9680,9 @@
       <c r="F42" s="74"/>
       <c r="G42" s="92"/>
       <c r="H42" s="74"/>
-      <c r="I42" s="25"/>
+      <c r="I42" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J42" s="67"/>
       <c r="K42" s="67"/>
       <c r="L42" s="67"/>
@@ -9644,7 +9705,9 @@
       <c r="F43" s="74"/>
       <c r="G43" s="92"/>
       <c r="H43" s="74"/>
-      <c r="I43" s="25"/>
+      <c r="I43" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J43" s="65"/>
       <c r="K43" s="65"/>
       <c r="L43" s="65"/>
@@ -9667,7 +9730,9 @@
       <c r="F44" s="74"/>
       <c r="G44" s="92"/>
       <c r="H44" s="74"/>
-      <c r="I44" s="25"/>
+      <c r="I44" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J44" s="65"/>
       <c r="K44" s="65"/>
       <c r="L44" s="65"/>
@@ -10042,7 +10107,7 @@
   <dimension ref="A1:T64"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD23"/>
+      <selection activeCell="I41" sqref="I41:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -10688,7 +10753,9 @@
         <v>141</v>
       </c>
       <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
+      <c r="I41" s="24" t="s">
+        <v>141</v>
+      </c>
       <c r="J41" s="24">
         <v>0</v>
       </c>
@@ -10718,7 +10785,9 @@
       <c r="F42" s="25"/>
       <c r="G42" s="86"/>
       <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
+      <c r="I42" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J42" s="21"/>
       <c r="K42" s="31"/>
       <c r="L42" s="21">
@@ -10748,7 +10817,9 @@
       <c r="H43" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I43" s="25"/>
+      <c r="I43" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J43" s="21"/>
       <c r="K43" s="31"/>
       <c r="L43" s="21"/>
@@ -10772,7 +10843,9 @@
       <c r="F44" s="82"/>
       <c r="G44" s="88"/>
       <c r="H44" s="82"/>
-      <c r="I44" s="25"/>
+      <c r="I44" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J44" s="21"/>
       <c r="K44" s="31"/>
       <c r="L44" s="21"/>
@@ -10798,7 +10871,9 @@
       <c r="F45" s="26"/>
       <c r="G45" s="87"/>
       <c r="H45" s="26"/>
-      <c r="I45" s="25"/>
+      <c r="I45" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J45" s="25"/>
       <c r="K45" s="32"/>
       <c r="L45" s="25"/>
@@ -10824,7 +10899,9 @@
       <c r="F46" s="26"/>
       <c r="G46" s="87"/>
       <c r="H46" s="26"/>
-      <c r="I46" s="25"/>
+      <c r="I46" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J46" s="21"/>
       <c r="K46" s="31"/>
       <c r="L46" s="21"/>
@@ -10848,7 +10925,9 @@
       <c r="F47" s="26"/>
       <c r="G47" s="87"/>
       <c r="H47" s="26"/>
-      <c r="I47" s="25"/>
+      <c r="I47" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J47" s="21"/>
       <c r="K47" s="31"/>
       <c r="L47" s="21"/>
@@ -11232,8 +11311,8 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38:I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -11836,7 +11915,9 @@
         <v>141</v>
       </c>
       <c r="H38" s="67"/>
-      <c r="I38" s="24"/>
+      <c r="I38" s="24" t="s">
+        <v>141</v>
+      </c>
       <c r="J38" s="67"/>
       <c r="K38" s="67"/>
       <c r="L38" s="67"/>
@@ -11861,7 +11942,9 @@
       <c r="F39" s="67"/>
       <c r="G39" s="90"/>
       <c r="H39" s="67"/>
-      <c r="I39" s="25"/>
+      <c r="I39" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J39" s="65"/>
       <c r="K39" s="65"/>
       <c r="L39" s="65"/>
@@ -11884,7 +11967,9 @@
       <c r="F40" s="70"/>
       <c r="G40" s="91"/>
       <c r="H40" s="70"/>
-      <c r="I40" s="25"/>
+      <c r="I40" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J40" s="65"/>
       <c r="K40" s="65"/>
       <c r="L40" s="65"/>
@@ -11907,7 +11992,9 @@
       <c r="F41" s="74"/>
       <c r="G41" s="94"/>
       <c r="H41" s="74"/>
-      <c r="I41" s="25"/>
+      <c r="I41" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J41" s="65"/>
       <c r="K41" s="65"/>
       <c r="L41" s="65"/>
@@ -11932,7 +12019,9 @@
       <c r="F42" s="74"/>
       <c r="G42" s="92"/>
       <c r="H42" s="74"/>
-      <c r="I42" s="25"/>
+      <c r="I42" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J42" s="67"/>
       <c r="K42" s="67"/>
       <c r="L42" s="67"/>
@@ -11955,7 +12044,9 @@
       <c r="F43" s="74"/>
       <c r="G43" s="92"/>
       <c r="H43" s="74"/>
-      <c r="I43" s="25"/>
+      <c r="I43" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J43" s="65"/>
       <c r="K43" s="65"/>
       <c r="L43" s="65"/>
@@ -11978,7 +12069,9 @@
       <c r="F44" s="74"/>
       <c r="G44" s="92"/>
       <c r="H44" s="74"/>
-      <c r="I44" s="25"/>
+      <c r="I44" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J44" s="65"/>
       <c r="K44" s="65"/>
       <c r="L44" s="65"/>
@@ -12352,8 +12445,8 @@
   </sheetPr>
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD23"/>
+    <sheetView topLeftCell="L7" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13005,7 +13098,9 @@
         <v>141</v>
       </c>
       <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
+      <c r="I41" s="24" t="s">
+        <v>141</v>
+      </c>
       <c r="J41" s="24">
         <v>0</v>
       </c>
@@ -13035,7 +13130,9 @@
       <c r="F42" s="25"/>
       <c r="G42" s="86"/>
       <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
+      <c r="I42" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J42" s="21"/>
       <c r="K42" s="31"/>
       <c r="L42" s="21">
@@ -13065,7 +13162,9 @@
       <c r="H43" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I43" s="25"/>
+      <c r="I43" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J43" s="21"/>
       <c r="K43" s="31"/>
       <c r="L43" s="21"/>
@@ -13089,7 +13188,9 @@
       <c r="F44" s="82"/>
       <c r="G44" s="88"/>
       <c r="H44" s="82"/>
-      <c r="I44" s="25"/>
+      <c r="I44" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J44" s="21"/>
       <c r="K44" s="31"/>
       <c r="L44" s="21"/>
@@ -13115,7 +13216,9 @@
       <c r="F45" s="26"/>
       <c r="G45" s="87"/>
       <c r="H45" s="26"/>
-      <c r="I45" s="25"/>
+      <c r="I45" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J45" s="25"/>
       <c r="K45" s="32"/>
       <c r="L45" s="25"/>
@@ -13141,7 +13244,9 @@
       <c r="F46" s="26"/>
       <c r="G46" s="87"/>
       <c r="H46" s="26"/>
-      <c r="I46" s="25"/>
+      <c r="I46" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J46" s="21"/>
       <c r="K46" s="31"/>
       <c r="L46" s="21"/>
@@ -13165,7 +13270,9 @@
       <c r="F47" s="26"/>
       <c r="G47" s="87"/>
       <c r="H47" s="26"/>
-      <c r="I47" s="25"/>
+      <c r="I47" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J47" s="21"/>
       <c r="K47" s="31"/>
       <c r="L47" s="21"/>
@@ -13550,7 +13657,7 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD20"/>
+      <selection activeCell="B31" sqref="B31:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -14153,7 +14260,9 @@
         <v>141</v>
       </c>
       <c r="H38" s="67"/>
-      <c r="I38" s="24"/>
+      <c r="I38" s="24" t="s">
+        <v>141</v>
+      </c>
       <c r="J38" s="67"/>
       <c r="K38" s="67"/>
       <c r="L38" s="67"/>
@@ -14178,7 +14287,9 @@
       <c r="F39" s="67"/>
       <c r="G39" s="90"/>
       <c r="H39" s="67"/>
-      <c r="I39" s="25"/>
+      <c r="I39" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J39" s="65"/>
       <c r="K39" s="65"/>
       <c r="L39" s="65"/>
@@ -14201,7 +14312,9 @@
       <c r="F40" s="70"/>
       <c r="G40" s="91"/>
       <c r="H40" s="70"/>
-      <c r="I40" s="25"/>
+      <c r="I40" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J40" s="65"/>
       <c r="K40" s="65"/>
       <c r="L40" s="65"/>
@@ -14224,7 +14337,9 @@
       <c r="F41" s="74"/>
       <c r="G41" s="94"/>
       <c r="H41" s="74"/>
-      <c r="I41" s="25"/>
+      <c r="I41" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J41" s="65"/>
       <c r="K41" s="65"/>
       <c r="L41" s="65"/>
@@ -14249,7 +14364,9 @@
       <c r="F42" s="74"/>
       <c r="G42" s="92"/>
       <c r="H42" s="74"/>
-      <c r="I42" s="25"/>
+      <c r="I42" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J42" s="67"/>
       <c r="K42" s="67"/>
       <c r="L42" s="67"/>
@@ -14272,7 +14389,9 @@
       <c r="F43" s="74"/>
       <c r="G43" s="92"/>
       <c r="H43" s="74"/>
-      <c r="I43" s="25"/>
+      <c r="I43" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J43" s="65"/>
       <c r="K43" s="65"/>
       <c r="L43" s="65"/>
@@ -14295,7 +14414,9 @@
       <c r="F44" s="74"/>
       <c r="G44" s="92"/>
       <c r="H44" s="74"/>
-      <c r="I44" s="25"/>
+      <c r="I44" s="25" t="s">
+        <v>141</v>
+      </c>
       <c r="J44" s="65"/>
       <c r="K44" s="65"/>
       <c r="L44" s="65"/>

</xml_diff>